<commit_message>
fix: powermonitor lower resistor to 680ohm
</commit_message>
<xml_diff>
--- a/docs/PowerMonitor.xlsx
+++ b/docs/PowerMonitor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Domoticata\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61B89986-18B2-401A-834D-DFAD88E777B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF880DA1-5849-4DA4-8335-1EFAEAA9BE27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="56">
   <si>
     <t>1.2</t>
   </si>
@@ -86,9 +86,6 @@
     <t>6.8</t>
   </si>
   <si>
-    <t>Bit ADC</t>
-  </si>
-  <si>
     <t>Ramo misurazione corrente</t>
   </si>
   <si>
@@ -143,18 +140,12 @@
     <t>Costanti fisse</t>
   </si>
   <si>
-    <t>bit</t>
-  </si>
-  <si>
     <t>Risoluzione ADC</t>
   </si>
   <si>
     <t>mV/step</t>
   </si>
   <si>
-    <t>Massimo valore ADC concesso</t>
-  </si>
-  <si>
     <t>Massima tensione ADC concessa</t>
   </si>
   <si>
@@ -170,9 +161,6 @@
     <t>Valori forniti</t>
   </si>
   <si>
-    <t>step</t>
-  </si>
-  <si>
     <t>steps</t>
   </si>
   <si>
@@ -191,9 +179,6 @@
     <t>VA/step</t>
   </si>
   <si>
-    <t>Valori ADC</t>
-  </si>
-  <si>
     <t>Massima tensione di rete tollerabile</t>
   </si>
   <si>
@@ -216,17 +201,27 @@
   </si>
   <si>
     <t>Massima potenza di rete</t>
+  </si>
+  <si>
+    <t>Valore ADC @ Massima tensione ADC</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -370,61 +365,67 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -644,791 +645,744 @@
   <dimension ref="B2:U1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:L16"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="31.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="10.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" style="2" customWidth="1"/>
-    <col min="6" max="6" width="30.75" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="30.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.875" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.5" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="26" width="7.625" style="2" customWidth="1"/>
-    <col min="27" max="16384" width="12.625" style="2"/>
+    <col min="1" max="1" width="10.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" style="1" customWidth="1"/>
+    <col min="6" max="6" width="30.75" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="30.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="26" width="7.625" style="1" customWidth="1"/>
+    <col min="27" max="16384" width="12.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-    </row>
+    <row r="2" spans="2:21" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B3" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="24"/>
-      <c r="F3" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="23"/>
-      <c r="H3" s="24"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="K3" s="23"/>
-      <c r="L3" s="24"/>
-      <c r="N3" s="3" t="s">
+      <c r="B3" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="20"/>
+      <c r="D3" s="21"/>
+      <c r="F3" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="20"/>
+      <c r="H3" s="21"/>
+      <c r="J3" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" s="20"/>
+      <c r="L3" s="21"/>
+      <c r="N3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="P3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="Q3" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>56</v>
+      <c r="Q3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="R3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="23">
         <v>230</v>
       </c>
-      <c r="D4" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" s="10"/>
-      <c r="F4" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="G4" s="11">
+      <c r="D4" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="4"/>
+      <c r="F4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="9">
         <f>$C$8-$G$5</f>
-        <v>9272.7818762178213</v>
-      </c>
-      <c r="H4" s="9" t="s">
+        <v>9310.3966067582787</v>
+      </c>
+      <c r="H4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="18"/>
-      <c r="J4" s="7" t="s">
+      <c r="J4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="K4" s="11">
-        <f>($C$18-$C$17)/(($C$5/$C$4)*$C$14*$C$7)</f>
-        <v>117.91005576285677</v>
-      </c>
-      <c r="L4" s="9" t="s">
+      <c r="K4" s="9">
+        <f>($C$17-$C$12)/(($C$5/$C$4)*$C$15*$C$7)</f>
+        <v>111.81125977512282</v>
+      </c>
+      <c r="L4" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="6">
+      <c r="N4" s="5">
         <v>1</v>
       </c>
-      <c r="O4" s="6">
+      <c r="O4" s="5">
         <v>10</v>
       </c>
-      <c r="P4" s="6">
+      <c r="P4" s="5">
         <v>100</v>
       </c>
-      <c r="Q4" s="6">
+      <c r="Q4" s="5">
         <v>1</v>
       </c>
-      <c r="R4" s="6">
+      <c r="R4" s="5">
         <v>10</v>
       </c>
-      <c r="S4" s="6">
+      <c r="S4" s="5">
         <v>100</v>
       </c>
-      <c r="T4" s="6">
+      <c r="T4" s="5">
         <v>1</v>
       </c>
-      <c r="U4" s="6">
+      <c r="U4" s="5">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="23">
         <v>4000</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G5" s="11">
-        <f>($C$18-$C$17)/(($C$4*$C$14*$C$6)/$C$8)</f>
-        <v>727.21812378217874</v>
-      </c>
-      <c r="H5" s="9" t="s">
+      <c r="F5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G5" s="9">
+        <f>($C$17-$C$12)/(($C$4*$C$15*$C$6)/$C$8)</f>
+        <v>689.60339324172139</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="18"/>
-      <c r="J5" s="7"/>
-      <c r="K5" s="8"/>
-      <c r="L5" s="9"/>
-      <c r="N5" s="6" t="s">
+      <c r="J5" s="6"/>
+      <c r="K5" s="7"/>
+      <c r="L5" s="8"/>
+      <c r="N5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="O5" s="6">
+      <c r="O5" s="5">
         <v>12</v>
       </c>
-      <c r="P5" s="6">
+      <c r="P5" s="5">
         <v>120</v>
       </c>
-      <c r="Q5" s="6" t="s">
+      <c r="Q5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="R5" s="6">
+      <c r="R5" s="5">
         <v>12</v>
       </c>
-      <c r="S5" s="6">
+      <c r="S5" s="5">
         <v>120</v>
       </c>
-      <c r="T5" s="6" t="s">
+      <c r="T5" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="U5" s="6">
+      <c r="U5" s="5">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B6" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="8">
+      <c r="B6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" s="23">
         <v>6.13E-2</v>
       </c>
-      <c r="D6" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="11"/>
-      <c r="H6" s="9"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="11"/>
-      <c r="L6" s="20"/>
-      <c r="N6" s="6" t="s">
+      <c r="D6" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="6"/>
+      <c r="G6" s="9"/>
+      <c r="H6" s="8"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="17"/>
+      <c r="N6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="O6" s="6">
+      <c r="O6" s="5">
         <v>15</v>
       </c>
-      <c r="P6" s="6">
+      <c r="P6" s="5">
         <v>150</v>
       </c>
-      <c r="Q6" s="6" t="s">
+      <c r="Q6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="R6" s="6">
+      <c r="R6" s="5">
         <v>15</v>
       </c>
-      <c r="S6" s="6">
+      <c r="S6" s="5">
         <v>150</v>
       </c>
-      <c r="T6" s="6" t="s">
+      <c r="T6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="U6" s="6">
+      <c r="U6" s="5">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="23">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="D7" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C7" s="8">
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G7" s="18"/>
-      <c r="H7" s="20"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="K7" s="18"/>
-      <c r="L7" s="20"/>
-      <c r="N7" s="6" t="s">
+      <c r="F7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H7" s="17"/>
+      <c r="J7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="L7" s="17"/>
+      <c r="N7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="O7" s="6">
+      <c r="O7" s="5">
         <v>18</v>
       </c>
-      <c r="P7" s="6">
+      <c r="P7" s="5">
         <v>180</v>
       </c>
-      <c r="Q7" s="6" t="s">
+      <c r="Q7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="R7" s="6">
+      <c r="R7" s="5">
         <v>18</v>
       </c>
-      <c r="S7" s="6">
+      <c r="S7" s="5">
         <v>180</v>
       </c>
-      <c r="T7" s="6" t="s">
+      <c r="T7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="U7" s="6">
+      <c r="U7" s="5">
         <v>18</v>
       </c>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B8" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="18">
+      <c r="B8" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="24">
         <v>10000</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="8">
+      <c r="F8" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="7">
         <v>10000</v>
       </c>
-      <c r="H8" s="9" t="s">
+      <c r="H8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I8" s="18"/>
-      <c r="J8" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="K8" s="18">
+      <c r="J8" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="K8" s="1">
         <v>120</v>
       </c>
-      <c r="L8" s="9" t="s">
+      <c r="L8" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="N8" s="6" t="s">
+      <c r="N8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="O8" s="6">
+      <c r="O8" s="5">
         <v>22</v>
       </c>
-      <c r="P8" s="6">
+      <c r="P8" s="5">
         <v>220</v>
       </c>
-      <c r="Q8" s="6" t="s">
+      <c r="Q8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="R8" s="6">
+      <c r="R8" s="5">
         <v>22</v>
       </c>
-      <c r="S8" s="6">
+      <c r="S8" s="5">
         <v>220</v>
       </c>
-      <c r="T8" s="6" t="s">
+      <c r="T8" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="U8" s="6">
+      <c r="U8" s="5">
         <v>22</v>
       </c>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B9" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="8">
-        <v>3.3</v>
-      </c>
-      <c r="D9" s="9" t="s">
+      <c r="B9" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="23">
+        <v>3</v>
+      </c>
+      <c r="D9" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="F9" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="8">
-        <v>820</v>
-      </c>
-      <c r="H9" s="9" t="s">
+      <c r="F9" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9" s="7">
+        <v>680</v>
+      </c>
+      <c r="H9" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="18"/>
-      <c r="J9" s="12"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="20"/>
-      <c r="N9" s="6" t="s">
+      <c r="J9" s="10"/>
+      <c r="L9" s="17"/>
+      <c r="N9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="O9" s="6">
+      <c r="O9" s="5">
         <v>27</v>
       </c>
-      <c r="P9" s="6">
+      <c r="P9" s="5">
         <v>270</v>
       </c>
-      <c r="Q9" s="6" t="s">
+      <c r="Q9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="R9" s="6">
+      <c r="R9" s="5">
         <v>27</v>
       </c>
-      <c r="S9" s="6">
+      <c r="S9" s="5">
         <v>270</v>
       </c>
-      <c r="T9" s="6" t="s">
+      <c r="T9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="U9" s="6" t="s">
-        <v>28</v>
+      <c r="U9" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B10" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="18">
-        <v>0.2</v>
-      </c>
-      <c r="D10" s="9" t="s">
+      <c r="B10" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="24">
+        <v>0</v>
+      </c>
+      <c r="D10" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="G10" s="18">
+      <c r="E10" s="4"/>
+      <c r="F10" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="1">
         <f>$G$8+$G$9</f>
-        <v>10820</v>
-      </c>
-      <c r="H10" s="9" t="s">
+        <v>10680</v>
+      </c>
+      <c r="H10" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I10" s="18"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="20"/>
-      <c r="N10" s="6" t="s">
+      <c r="J10" s="10"/>
+      <c r="L10" s="17"/>
+      <c r="N10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="O10" s="6">
+      <c r="O10" s="5">
         <v>33</v>
       </c>
-      <c r="P10" s="6">
+      <c r="P10" s="5">
         <v>330</v>
       </c>
-      <c r="Q10" s="6" t="s">
+      <c r="Q10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="R10" s="6">
+      <c r="R10" s="5">
         <v>33</v>
       </c>
-      <c r="S10" s="6">
+      <c r="S10" s="5">
         <v>330</v>
       </c>
-      <c r="T10" s="6" t="s">
+      <c r="T10" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="U10" s="6" t="s">
-        <v>28</v>
+      <c r="U10" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B11" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11" s="19">
-        <v>12</v>
-      </c>
-      <c r="D11" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="F11" s="12"/>
-      <c r="G11" s="18"/>
-      <c r="H11" s="20"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="18"/>
-      <c r="L11" s="20"/>
-      <c r="N11" s="6" t="s">
+      <c r="B11" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="C11" s="24">
+        <v>3840</v>
+      </c>
+      <c r="D11" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="F11" s="10"/>
+      <c r="H11" s="17"/>
+      <c r="J11" s="10"/>
+      <c r="L11" s="17"/>
+      <c r="N11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="O11" s="6">
+      <c r="O11" s="5">
         <v>39</v>
       </c>
-      <c r="P11" s="6">
+      <c r="P11" s="5">
         <v>390</v>
       </c>
-      <c r="Q11" s="6" t="s">
+      <c r="Q11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="R11" s="6">
+      <c r="R11" s="5">
         <v>39</v>
       </c>
-      <c r="S11" s="6">
+      <c r="S11" s="5">
         <v>390</v>
       </c>
-      <c r="T11" s="6" t="s">
+      <c r="T11" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="U11" s="6" t="s">
-        <v>28</v>
+      <c r="U11" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="F12" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="G12" s="18">
-        <f>((($G$8+$G$9)*($C$18-$C$17)/$G$9)/$C$6)/$C$14</f>
-        <v>220.70183205418653</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="J12" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="K12" s="18">
-        <f>((($C$18-$C$17)/$K$8)/$C$7)/$C$14</f>
-        <v>17.088413878674892</v>
-      </c>
-      <c r="L12" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="N12" s="6" t="s">
+      <c r="B12" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C12" s="16">
+        <v>1.625</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="G12" s="1">
+        <f>((($G$8+$G$9)*($C$17-$C$12)/$G$9)/$C$6)/$C$15</f>
+        <v>249.10908458220058</v>
+      </c>
+      <c r="H12" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="K12" s="1">
+        <f>((($C$17-$C$12)/$K$8)/$C$7)/$C$15</f>
+        <v>16.204530402191711</v>
+      </c>
+      <c r="L12" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="N12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="O12" s="6">
+      <c r="O12" s="5">
         <v>47</v>
       </c>
-      <c r="P12" s="6">
+      <c r="P12" s="5">
         <v>470</v>
       </c>
-      <c r="Q12" s="6" t="s">
+      <c r="Q12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="R12" s="6">
+      <c r="R12" s="5">
         <v>47</v>
       </c>
-      <c r="S12" s="6">
+      <c r="S12" s="5">
         <v>470</v>
       </c>
-      <c r="T12" s="6" t="s">
+      <c r="T12" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="U12" s="6" t="s">
-        <v>28</v>
+      <c r="U12" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B13" s="22" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="23"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
       <c r="D13" s="24"/>
-      <c r="F13" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="G13" s="18">
-        <f>((($G$8+$G$9)*($C$9-$C$17)/$G$9)/$C$6)/$C$14</f>
-        <v>251.14346406166064</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="J13" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="K13" s="18">
-        <f>((($C$9-$C$17)/$K$8)/$C$7)/$C$14</f>
-        <v>19.445436482630054</v>
-      </c>
-      <c r="L13" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="N13" s="6" t="s">
+      <c r="F13" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="1">
+        <f>((($G$8+$G$9)*($C$9-$C$12)/$G$9)/$C$6)/$C$15</f>
+        <v>249.10908458220058</v>
+      </c>
+      <c r="H13" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="K13" s="1">
+        <f>((($C$9-$C$12)/$K$8)/$C$7)/$C$15</f>
+        <v>16.204530402191711</v>
+      </c>
+      <c r="L13" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="N13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="O13" s="6">
+      <c r="O13" s="5">
         <v>56</v>
       </c>
-      <c r="P13" s="6">
+      <c r="P13" s="5">
         <v>560</v>
       </c>
-      <c r="Q13" s="6" t="s">
+      <c r="Q13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="R13" s="6">
+      <c r="R13" s="5">
         <v>56</v>
       </c>
-      <c r="S13" s="6">
+      <c r="S13" s="5">
         <v>560</v>
       </c>
-      <c r="T13" s="6" t="s">
+      <c r="T13" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="U13" s="6" t="s">
-        <v>28</v>
+      <c r="U13" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B14" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="18">
+      <c r="B14" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C14" s="20"/>
+      <c r="D14" s="21"/>
+      <c r="F14" s="10"/>
+      <c r="H14" s="17"/>
+      <c r="J14" s="10"/>
+      <c r="L14" s="17"/>
+      <c r="N14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="O14" s="5">
+        <v>68</v>
+      </c>
+      <c r="P14" s="5">
+        <v>680</v>
+      </c>
+      <c r="Q14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="R14" s="5">
+        <v>68</v>
+      </c>
+      <c r="S14" s="5">
+        <v>680</v>
+      </c>
+      <c r="T14" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="U14" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="24">
         <f>SQRT(2)</f>
         <v>1.4142135623730951</v>
       </c>
-      <c r="D14" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="F14" s="12"/>
-      <c r="G14" s="18"/>
-      <c r="H14" s="20"/>
-      <c r="J14" s="12"/>
-      <c r="K14" s="18"/>
-      <c r="L14" s="20"/>
-      <c r="N14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="O14" s="6">
-        <v>68</v>
-      </c>
-      <c r="P14" s="6">
-        <v>680</v>
-      </c>
-      <c r="Q14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="R14" s="6">
-        <v>68</v>
-      </c>
-      <c r="S14" s="6">
-        <v>680</v>
-      </c>
-      <c r="T14" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="U14" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="15" spans="2:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="18">
-        <f>POWER(2,$C$11)</f>
-        <v>4096</v>
-      </c>
-      <c r="D15" s="20" t="s">
-        <v>45</v>
-      </c>
-      <c r="F15" s="12" t="s">
+      <c r="D15" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="G15" s="1">
+        <f>($G$13*1000)/$C$11</f>
+        <v>64.872157443281409</v>
+      </c>
+      <c r="H15" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="18">
-        <f>($G$13*1000)/$C$15</f>
-        <v>61.314322280678866</v>
-      </c>
-      <c r="H15" s="20" t="s">
-        <v>25</v>
-      </c>
-      <c r="J15" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="K15" s="18">
+      <c r="J15" s="26" t="s">
+        <v>54</v>
+      </c>
+      <c r="K15" s="1">
         <f>$K$12*$C$4</f>
-        <v>3930.335192095225</v>
-      </c>
-      <c r="L15" s="9" t="s">
+        <v>3727.0419925040937</v>
+      </c>
+      <c r="L15" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="N15" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="O15" s="6">
+      <c r="N15" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="O15" s="5">
         <v>82</v>
       </c>
-      <c r="P15" s="6">
+      <c r="P15" s="5">
         <v>820</v>
       </c>
-      <c r="Q15" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="R15" s="6">
+      <c r="Q15" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="R15" s="5">
         <v>82</v>
       </c>
-      <c r="S15" s="6">
+      <c r="S15" s="5">
         <v>820</v>
       </c>
-      <c r="T15" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="U15" s="6" t="s">
-        <v>28</v>
+      <c r="T15" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="U15" s="5" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="16" spans="2:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="C16" s="18">
-        <f>($C$9*1000)/$C$15</f>
-        <v>0.8056640625</v>
-      </c>
-      <c r="D16" s="20" t="s">
-        <v>37</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="18">
-        <f>($K$13*1000)/$C$15</f>
-        <v>4.7474210162671033</v>
-      </c>
-      <c r="H16" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="J16" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="K16" s="19">
+      <c r="B16" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="24">
+        <f>($C$9*1000)/$C$11</f>
+        <v>0.78125</v>
+      </c>
+      <c r="D16" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="1">
+        <f>($K$13*1000)/$C$11</f>
+        <v>4.2199297922374246</v>
+      </c>
+      <c r="H16" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="K16" s="16">
         <f>$K$13*$C$4</f>
-        <v>4472.4503910049125</v>
-      </c>
-      <c r="L16" s="14" t="s">
+        <v>3727.0419925040937</v>
+      </c>
+      <c r="L16" s="12" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" s="18">
-        <f>$C$9/2</f>
-        <v>1.65</v>
-      </c>
-      <c r="D17" s="20" t="s">
+      <c r="B17" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="16">
+        <f>$C$9-$C$10</f>
+        <v>3</v>
+      </c>
+      <c r="D17" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="F17" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="G17" s="19">
-        <f>$K$16/$C$15</f>
-        <v>1.0919068337414337</v>
-      </c>
-      <c r="H17" s="14" t="s">
-        <v>50</v>
+      <c r="F17" s="13" t="s">
+        <v>45</v>
+      </c>
+      <c r="G17" s="16">
+        <f>$K$16/$C$11</f>
+        <v>0.97058385221460775</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="C18" s="18">
-        <f>$C$9-$C$10</f>
-        <v>3.0999999999999996</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>1</v>
-      </c>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="C19" s="19">
-        <f>ROUND($C$18/($C$16/1000),0)</f>
-        <v>3848</v>
-      </c>
-      <c r="D19" s="21" t="s">
-        <v>44</v>
-      </c>
-    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25"/>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="18"/>
-      <c r="C20" s="18"/>
-      <c r="D20" s="16"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
+      <c r="D20" s="25"/>
     </row>
     <row r="21" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="5"/>
-      <c r="C22" s="18"/>
-      <c r="D22" s="18"/>
+      <c r="B22" s="4"/>
     </row>
     <row r="23" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="18"/>
-      <c r="D23" s="16"/>
+      <c r="D23" s="14"/>
     </row>
     <row r="24" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="18"/>
-      <c r="C24" s="18"/>
-      <c r="D24" s="16"/>
+      <c r="D24" s="14"/>
     </row>
     <row r="25" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="18"/>
-      <c r="D25" s="16"/>
+      <c r="D25" s="14"/>
     </row>
-    <row r="26" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="18"/>
-    </row>
+    <row r="26" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="28" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="29" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="30" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="31" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="32" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="16"/>
-      <c r="C45" s="17"/>
-      <c r="D45" s="18"/>
+    <row r="33" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="14"/>
+      <c r="C45" s="15"/>
     </row>
-    <row r="46" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="16"/>
-      <c r="C46" s="17"/>
-      <c r="D46" s="18"/>
+    <row r="46" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="14"/>
+      <c r="C46" s="15"/>
     </row>
-    <row r="47" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2386,7 +2340,7 @@
     <mergeCell ref="J3:L3"/>
     <mergeCell ref="F3:H3"/>
     <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B14:D14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
!feat: added sampling frequency calculator section.
</commit_message>
<xml_diff>
--- a/docs/PowerMonitor.xlsx
+++ b/docs/PowerMonitor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Domoticata\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF880DA1-5849-4DA4-8335-1EFAEAA9BE27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36F10D0E-2A70-48ED-888F-055370841F29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="130" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="73">
   <si>
     <t>1.2</t>
   </si>
@@ -204,13 +204,64 @@
   </si>
   <si>
     <t>Valore ADC @ Massima tensione ADC</t>
+  </si>
+  <si>
+    <t>CALCOLO FREQUENZA DI CAMPIONAMENTO OTTIMALE</t>
+  </si>
+  <si>
+    <t>CALCOLO COSTANTI DI LIBRERIA</t>
+  </si>
+  <si>
+    <t>Frequenza di rete</t>
+  </si>
+  <si>
+    <t>Hz</t>
+  </si>
+  <si>
+    <t>Frequenza di campionamento</t>
+  </si>
+  <si>
+    <t>Numero totale di campioni</t>
+  </si>
+  <si>
+    <t>samples</t>
+  </si>
+  <si>
+    <t>Num. cicli frequenza di rete acquisiti</t>
+  </si>
+  <si>
+    <t>cicli</t>
+  </si>
+  <si>
+    <t>Risultato</t>
+  </si>
+  <si>
+    <t>bytes</t>
+  </si>
+  <si>
+    <t>Memoria buffer richiesta</t>
+  </si>
+  <si>
+    <t>Tempo di acquisizione campioni</t>
+  </si>
+  <si>
+    <t>ms</t>
+  </si>
+  <si>
+    <t>Numero di bytes per campione</t>
+  </si>
+  <si>
+    <t>Numero di canali</t>
+  </si>
+  <si>
+    <t>Nota: acquisire almeno 10 cicli per avere letture stabili.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -231,14 +282,27 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -247,14 +311,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF6666"/>
-        <bgColor rgb="FFFF6666"/>
+        <fgColor rgb="FFFFFFCC"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00FFFF"/>
-        <bgColor rgb="FF00FFFF"/>
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -263,52 +332,6 @@
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -361,75 +384,160 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Nota" xfId="1" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -642,11 +750,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:U1000"/>
+  <dimension ref="B2:U1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -665,702 +771,820 @@
     <col min="27" max="16384" width="12.625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:21" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B3" s="19" t="s">
+    <row r="2" spans="2:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+      <c r="S2" s="19"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="19"/>
+    </row>
+    <row r="3" spans="2:21" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B4" s="31" t="s">
         <v>33</v>
       </c>
-      <c r="C3" s="20"/>
-      <c r="D3" s="21"/>
-      <c r="F3" s="19" t="s">
+      <c r="C4" s="32"/>
+      <c r="D4" s="33"/>
+      <c r="F4" s="31" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="20"/>
-      <c r="H3" s="21"/>
-      <c r="J3" s="19" t="s">
+      <c r="G4" s="32"/>
+      <c r="H4" s="33"/>
+      <c r="J4" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="K3" s="20"/>
-      <c r="L3" s="21"/>
-      <c r="N3" s="2" t="s">
+      <c r="K4" s="32"/>
+      <c r="L4" s="33"/>
+      <c r="N4" s="31" t="s">
         <v>10</v>
       </c>
-      <c r="O3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="Q3" s="2" t="s">
+      <c r="O4" s="32"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="R3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="T3" s="2" t="s">
+      <c r="R4" s="32"/>
+      <c r="S4" s="33"/>
+      <c r="T4" s="32" t="s">
         <v>51</v>
       </c>
-      <c r="U3" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B4" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="23">
-        <v>230</v>
-      </c>
-      <c r="D4" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" s="4"/>
-      <c r="F4" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" s="9">
-        <f>$C$8-$G$5</f>
-        <v>9310.3966067582787</v>
-      </c>
-      <c r="H4" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="K4" s="9">
-        <f>($C$17-$C$12)/(($C$5/$C$4)*$C$15*$C$7)</f>
-        <v>111.81125977512282</v>
-      </c>
-      <c r="L4" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="N4" s="5">
-        <v>1</v>
-      </c>
-      <c r="O4" s="5">
-        <v>10</v>
-      </c>
-      <c r="P4" s="5">
-        <v>100</v>
-      </c>
-      <c r="Q4" s="5">
-        <v>1</v>
-      </c>
-      <c r="R4" s="5">
-        <v>10</v>
-      </c>
-      <c r="S4" s="5">
-        <v>100</v>
-      </c>
-      <c r="T4" s="5">
-        <v>1</v>
-      </c>
-      <c r="U4" s="5">
-        <v>10</v>
-      </c>
+      <c r="U4" s="33"/>
     </row>
     <row r="5" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="23">
-        <v>4000</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="9">
-        <f>($C$17-$C$12)/(($C$4*$C$15*$C$6)/$C$8)</f>
-        <v>689.60339324172139</v>
-      </c>
-      <c r="H5" s="8" t="s">
+      <c r="B5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="5">
+        <v>230</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="7">
+        <f>$C$9-$G$6</f>
+        <v>9310.3966067582787</v>
+      </c>
+      <c r="H5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="6"/>
-      <c r="K5" s="7"/>
-      <c r="L5" s="8"/>
-      <c r="N5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="O5" s="5">
-        <v>12</v>
-      </c>
-      <c r="P5" s="5">
-        <v>120</v>
-      </c>
-      <c r="Q5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="R5" s="5">
-        <v>12</v>
-      </c>
-      <c r="S5" s="5">
-        <v>120</v>
-      </c>
-      <c r="T5" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="U5" s="5">
-        <v>12</v>
+      <c r="J5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="7">
+        <f>($C$18-$C$13)/(($C$6/$C$5)*$C$16*$C$8)</f>
+        <v>111.81125977512282</v>
+      </c>
+      <c r="L5" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N5" s="2">
+        <v>1</v>
+      </c>
+      <c r="O5" s="38">
+        <v>10</v>
+      </c>
+      <c r="P5" s="38">
+        <v>100</v>
+      </c>
+      <c r="Q5" s="2">
+        <v>1</v>
+      </c>
+      <c r="R5" s="38">
+        <v>10</v>
+      </c>
+      <c r="S5" s="20">
+        <v>100</v>
+      </c>
+      <c r="T5" s="38">
+        <v>1</v>
+      </c>
+      <c r="U5" s="20">
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B6" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" s="23">
-        <v>6.13E-2</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="8"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="17"/>
-      <c r="N6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="O6" s="5">
-        <v>15</v>
-      </c>
-      <c r="P6" s="5">
-        <v>150</v>
-      </c>
-      <c r="Q6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="R6" s="5">
-        <v>15</v>
-      </c>
-      <c r="S6" s="5">
-        <v>150</v>
-      </c>
-      <c r="T6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="U6" s="5">
-        <v>15</v>
+      <c r="B6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="5">
+        <v>4000</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G6" s="7">
+        <f>($C$18-$C$13)/(($C$5*$C$16*$C$7)/$C$9)</f>
+        <v>689.60339324172139</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="4"/>
+      <c r="K6" s="5"/>
+      <c r="L6" s="6"/>
+      <c r="N6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="O6" s="38">
+        <v>12</v>
+      </c>
+      <c r="P6" s="38">
+        <v>120</v>
+      </c>
+      <c r="Q6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="R6" s="38">
+        <v>12</v>
+      </c>
+      <c r="S6" s="20">
+        <v>120</v>
+      </c>
+      <c r="T6" s="38" t="s">
+        <v>0</v>
+      </c>
+      <c r="U6" s="20">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B7" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="23">
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="D7" s="8" t="s">
+      <c r="B7" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="5">
+        <v>6.13E-2</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="H7" s="17"/>
-      <c r="J7" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="L7" s="17"/>
-      <c r="N7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="O7" s="5">
-        <v>18</v>
-      </c>
-      <c r="P7" s="5">
-        <v>180</v>
-      </c>
-      <c r="Q7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="R7" s="5">
-        <v>18</v>
-      </c>
-      <c r="S7" s="5">
-        <v>180</v>
-      </c>
-      <c r="T7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="U7" s="5">
-        <v>18</v>
+      <c r="F7" s="4"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="6"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="7"/>
+      <c r="L7" s="15"/>
+      <c r="N7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="O7" s="38">
+        <v>15</v>
+      </c>
+      <c r="P7" s="38">
+        <v>150</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="R7" s="38">
+        <v>15</v>
+      </c>
+      <c r="S7" s="20">
+        <v>150</v>
+      </c>
+      <c r="T7" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="U7" s="20">
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B8" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="24">
-        <v>10000</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="G8" s="7">
-        <v>10000</v>
-      </c>
-      <c r="H8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="J8" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="K8" s="1">
-        <v>120</v>
-      </c>
-      <c r="L8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="N8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="O8" s="5">
-        <v>22</v>
-      </c>
-      <c r="P8" s="5">
-        <v>220</v>
-      </c>
-      <c r="Q8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="R8" s="5">
-        <v>22</v>
-      </c>
-      <c r="S8" s="5">
-        <v>220</v>
-      </c>
-      <c r="T8" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="U8" s="5">
-        <v>22</v>
+      <c r="B8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="5">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="F8" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" s="36"/>
+      <c r="H8" s="37"/>
+      <c r="J8" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" s="36"/>
+      <c r="L8" s="37"/>
+      <c r="N8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="O8" s="38">
+        <v>18</v>
+      </c>
+      <c r="P8" s="38">
+        <v>180</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="R8" s="38">
+        <v>18</v>
+      </c>
+      <c r="S8" s="20">
+        <v>180</v>
+      </c>
+      <c r="T8" s="38" t="s">
+        <v>5</v>
+      </c>
+      <c r="U8" s="20">
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B9" s="10" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="23">
-        <v>3</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="7">
-        <v>680</v>
-      </c>
-      <c r="H9" s="8" t="s">
+      <c r="B9" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="1">
+        <v>10000</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="10"/>
-      <c r="L9" s="17"/>
-      <c r="N9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="O9" s="5">
-        <v>27</v>
-      </c>
-      <c r="P9" s="5">
-        <v>270</v>
-      </c>
-      <c r="Q9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="R9" s="5">
-        <v>27</v>
-      </c>
-      <c r="S9" s="5">
-        <v>270</v>
-      </c>
-      <c r="T9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="U9" s="5" t="s">
-        <v>27</v>
+      <c r="F9" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="5">
+        <v>10000</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9" s="1">
+        <v>120</v>
+      </c>
+      <c r="L9" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="O9" s="38">
+        <v>22</v>
+      </c>
+      <c r="P9" s="38">
+        <v>220</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="R9" s="38">
+        <v>22</v>
+      </c>
+      <c r="S9" s="20">
+        <v>220</v>
+      </c>
+      <c r="T9" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="U9" s="20">
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B10" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" s="24">
-        <v>0</v>
-      </c>
-      <c r="D10" s="8" t="s">
+      <c r="B10" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="5">
+        <v>3</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="4"/>
-      <c r="F10" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="G10" s="1">
-        <f>$G$8+$G$9</f>
-        <v>10680</v>
-      </c>
-      <c r="H10" s="8" t="s">
+      <c r="F10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10" s="5">
+        <v>680</v>
+      </c>
+      <c r="H10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="J10" s="10"/>
-      <c r="L10" s="17"/>
-      <c r="N10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="O10" s="5">
-        <v>33</v>
-      </c>
-      <c r="P10" s="5">
-        <v>330</v>
-      </c>
-      <c r="Q10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="R10" s="5">
-        <v>33</v>
-      </c>
-      <c r="S10" s="5">
-        <v>330</v>
-      </c>
-      <c r="T10" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="U10" s="5" t="s">
+      <c r="J10" s="8"/>
+      <c r="L10" s="15"/>
+      <c r="N10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="O10" s="38">
+        <v>27</v>
+      </c>
+      <c r="P10" s="38">
+        <v>270</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="R10" s="38">
+        <v>27</v>
+      </c>
+      <c r="S10" s="20">
+        <v>270</v>
+      </c>
+      <c r="T10" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="U10" s="20" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B11" s="22" t="s">
-        <v>55</v>
-      </c>
-      <c r="C11" s="24">
-        <v>3840</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="F11" s="10"/>
-      <c r="H11" s="17"/>
-      <c r="J11" s="10"/>
-      <c r="L11" s="17"/>
-      <c r="N11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="O11" s="5">
-        <v>39</v>
-      </c>
-      <c r="P11" s="5">
-        <v>390</v>
-      </c>
-      <c r="Q11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="R11" s="5">
-        <v>39</v>
-      </c>
-      <c r="S11" s="5">
-        <v>390</v>
-      </c>
-      <c r="T11" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="U11" s="5" t="s">
+      <c r="B11" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3"/>
+      <c r="F11" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" s="1">
+        <f>$G$9+$G$10</f>
+        <v>10680</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="8"/>
+      <c r="L11" s="15"/>
+      <c r="N11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O11" s="38">
+        <v>33</v>
+      </c>
+      <c r="P11" s="38">
+        <v>330</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="R11" s="38">
+        <v>33</v>
+      </c>
+      <c r="S11" s="20">
+        <v>330</v>
+      </c>
+      <c r="T11" s="38" t="s">
+        <v>8</v>
+      </c>
+      <c r="U11" s="20" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B12" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="C12" s="16">
-        <v>1.625</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="G12" s="1">
-        <f>((($G$8+$G$9)*($C$17-$C$12)/$G$9)/$C$6)/$C$15</f>
-        <v>249.10908458220058</v>
-      </c>
-      <c r="H12" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J12" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="K12" s="1">
-        <f>((($C$17-$C$12)/$K$8)/$C$7)/$C$15</f>
-        <v>16.204530402191711</v>
-      </c>
-      <c r="L12" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="N12" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="O12" s="5">
-        <v>47</v>
-      </c>
-      <c r="P12" s="5">
-        <v>470</v>
-      </c>
-      <c r="Q12" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="R12" s="5">
-        <v>47</v>
-      </c>
-      <c r="S12" s="5">
-        <v>470</v>
-      </c>
-      <c r="T12" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="U12" s="5" t="s">
+      <c r="B12" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="1">
+        <v>3840</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="F12" s="8"/>
+      <c r="H12" s="15"/>
+      <c r="J12" s="8"/>
+      <c r="L12" s="15"/>
+      <c r="N12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="O12" s="38">
+        <v>39</v>
+      </c>
+      <c r="P12" s="38">
+        <v>390</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="R12" s="38">
+        <v>39</v>
+      </c>
+      <c r="S12" s="20">
+        <v>390</v>
+      </c>
+      <c r="T12" s="38" t="s">
+        <v>9</v>
+      </c>
+      <c r="U12" s="20" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="F13" s="10" t="s">
+      <c r="B13" s="11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="14">
+        <v>1.625</v>
+      </c>
+      <c r="D13" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="G13" s="1">
+        <f>((($G$9+$G$10)*($C$18-$C$13)/$G$10)/$C$7)/$C$16</f>
+        <v>249.10908458220058</v>
+      </c>
+      <c r="H13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J13" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="K13" s="1">
+        <f>((($C$18-$C$13)/$K$9)/$C$8)/$C$16</f>
+        <v>16.204530402191711</v>
+      </c>
+      <c r="L13" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="O13" s="38">
         <v>47</v>
       </c>
-      <c r="G13" s="1">
-        <f>((($G$8+$G$9)*($C$9-$C$12)/$G$9)/$C$6)/$C$15</f>
-        <v>249.10908458220058</v>
-      </c>
-      <c r="H13" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="J13" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="K13" s="1">
-        <f>((($C$9-$C$12)/$K$8)/$C$7)/$C$15</f>
-        <v>16.204530402191711</v>
-      </c>
-      <c r="L13" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="N13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="O13" s="5">
-        <v>56</v>
-      </c>
-      <c r="P13" s="5">
-        <v>560</v>
-      </c>
-      <c r="Q13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="R13" s="5">
-        <v>56</v>
-      </c>
-      <c r="S13" s="5">
-        <v>560</v>
-      </c>
-      <c r="T13" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="U13" s="5" t="s">
+      <c r="P13" s="38">
+        <v>470</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="R13" s="38">
+        <v>47</v>
+      </c>
+      <c r="S13" s="20">
+        <v>470</v>
+      </c>
+      <c r="T13" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="U13" s="20" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B14" s="19" t="s">
+      <c r="F14" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="G14" s="1">
+        <f>((($G$9+$G$10)*($C$10-$C$13)/$G$10)/$C$7)/$C$16</f>
+        <v>249.10908458220058</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J14" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="K14" s="1">
+        <f>((($C$10-$C$13)/$K$9)/$C$8)/$C$16</f>
+        <v>16.204530402191711</v>
+      </c>
+      <c r="L14" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O14" s="38">
+        <v>56</v>
+      </c>
+      <c r="P14" s="38">
+        <v>560</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="R14" s="38">
+        <v>56</v>
+      </c>
+      <c r="S14" s="20">
+        <v>560</v>
+      </c>
+      <c r="T14" s="38" t="s">
+        <v>13</v>
+      </c>
+      <c r="U14" s="20" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B15" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="21"/>
-      <c r="F14" s="10"/>
-      <c r="H14" s="17"/>
-      <c r="J14" s="10"/>
-      <c r="L14" s="17"/>
-      <c r="N14" s="5" t="s">
+      <c r="C15" s="32"/>
+      <c r="D15" s="33"/>
+      <c r="F15" s="8"/>
+      <c r="H15" s="15"/>
+      <c r="J15" s="8"/>
+      <c r="L15" s="15"/>
+      <c r="N15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="O14" s="5">
+      <c r="O15" s="38">
         <v>68</v>
       </c>
-      <c r="P14" s="5">
+      <c r="P15" s="38">
         <v>680</v>
       </c>
-      <c r="Q14" s="5" t="s">
+      <c r="Q15" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="R14" s="5">
+      <c r="R15" s="38">
         <v>68</v>
       </c>
-      <c r="S14" s="5">
+      <c r="S15" s="20">
         <v>680</v>
       </c>
-      <c r="T14" s="5" t="s">
+      <c r="T15" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="U14" s="5" t="s">
+      <c r="U15" s="20" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="2:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="10" t="s">
+    <row r="16" spans="2:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="24">
+      <c r="C16" s="1">
         <f>SQRT(2)</f>
         <v>1.4142135623730951</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="D16" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="F15" s="10" t="s">
+      <c r="F16" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="1">
-        <f>($G$13*1000)/$C$11</f>
+      <c r="G16" s="1">
+        <f>($G$14*1000)/$C$12</f>
         <v>64.872157443281409</v>
       </c>
-      <c r="H15" s="17" t="s">
+      <c r="H16" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="J15" s="26" t="s">
+      <c r="J16" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="K15" s="1">
-        <f>$K$12*$C$4</f>
+      <c r="K16" s="1">
+        <f>$K$13*$C$5</f>
         <v>3727.0419925040937</v>
       </c>
-      <c r="L15" s="8" t="s">
+      <c r="L16" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="N15" s="5" t="s">
+      <c r="N16" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="O15" s="5">
+      <c r="O16" s="40">
         <v>82</v>
       </c>
-      <c r="P15" s="5">
+      <c r="P16" s="40">
         <v>820</v>
       </c>
-      <c r="Q15" s="5" t="s">
+      <c r="Q16" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="R15" s="5">
+      <c r="R16" s="40">
         <v>82</v>
       </c>
-      <c r="S15" s="5">
+      <c r="S16" s="41">
         <v>820</v>
       </c>
-      <c r="T15" s="5" t="s">
+      <c r="T16" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="U15" s="5" t="s">
+      <c r="U16" s="41" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="2:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="10" t="s">
+    <row r="17" spans="2:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="24">
-        <f>($C$9*1000)/$C$11</f>
+      <c r="C17" s="1">
+        <f>($C$10*1000)/$C$12</f>
         <v>0.78125</v>
       </c>
-      <c r="D16" s="17" t="s">
+      <c r="D17" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="F16" s="10" t="s">
+      <c r="F17" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="1">
-        <f>($K$13*1000)/$C$11</f>
+      <c r="G17" s="1">
+        <f>($K$14*1000)/$C$12</f>
         <v>4.2199297922374246</v>
       </c>
-      <c r="H16" s="8" t="s">
+      <c r="H17" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="J16" s="11" t="s">
+      <c r="J17" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="K16" s="16">
-        <f>$K$13*$C$4</f>
+      <c r="K17" s="14">
+        <f>$K$14*$C$5</f>
         <v>3727.0419925040937</v>
       </c>
-      <c r="L16" s="12" t="s">
+      <c r="L17" s="10" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="13" t="s">
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B18" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="16">
-        <f>$C$9-$C$10</f>
+      <c r="C18" s="14">
+        <f>$C$10-$C$11</f>
         <v>3</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D18" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F18" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="G17" s="16">
-        <f>$K$16/$C$11</f>
+      <c r="G18" s="14">
+        <f>$K$17/$C$12</f>
         <v>0.97058385221460775</v>
       </c>
-      <c r="H17" s="12" t="s">
+      <c r="H18" s="10" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="24"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="B20" s="19" t="s">
+        <v>56</v>
+      </c>
+      <c r="C20" s="19"/>
+      <c r="D20" s="19"/>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19"/>
+      <c r="I20" s="19"/>
+      <c r="J20" s="19"/>
+      <c r="K20" s="19"/>
+      <c r="L20" s="19"/>
+      <c r="M20" s="19"/>
+      <c r="N20" s="19"/>
+      <c r="O20" s="19"/>
+      <c r="P20" s="19"/>
+      <c r="Q20" s="19"/>
+      <c r="R20" s="19"/>
+      <c r="S20" s="19"/>
+      <c r="T20" s="19"/>
+      <c r="U20" s="19"/>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="24"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="25"/>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="D21" s="12"/>
     </row>
-    <row r="21" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="4"/>
+    <row r="22" spans="2:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="31" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="32"/>
+      <c r="D22" s="33"/>
+      <c r="F22" s="34" t="s">
+        <v>65</v>
+      </c>
+      <c r="G22" s="32"/>
+      <c r="H22" s="33"/>
     </row>
-    <row r="23" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D23" s="14"/>
+    <row r="23" spans="2:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="22">
+        <v>50</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>59</v>
+      </c>
+      <c r="F23" s="28" t="s">
+        <v>63</v>
+      </c>
+      <c r="G23" s="22">
+        <f>$C$25/($C$24/$C$23)</f>
+        <v>10</v>
+      </c>
+      <c r="H23" s="23" t="s">
+        <v>64</v>
+      </c>
+      <c r="J23" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="K23" s="30"/>
+      <c r="L23" s="30"/>
     </row>
-    <row r="24" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D24" s="14"/>
+    <row r="24" spans="2:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C24" s="22">
+        <v>20000</v>
+      </c>
+      <c r="D24" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="F24" s="28" t="s">
+        <v>68</v>
+      </c>
+      <c r="G24" s="22">
+        <f>$G$23/$C$23*1000</f>
+        <v>200</v>
+      </c>
+      <c r="H24" s="23" t="s">
+        <v>69</v>
+      </c>
     </row>
-    <row r="25" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D25" s="14"/>
+    <row r="25" spans="2:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="28" t="s">
+        <v>61</v>
+      </c>
+      <c r="C25" s="22">
+        <v>4000</v>
+      </c>
+      <c r="D25" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="F25" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="G25" s="14">
+        <f>$C$25*$C$26*$C$27</f>
+        <v>16000</v>
+      </c>
+      <c r="H25" s="29" t="s">
+        <v>66</v>
+      </c>
+      <c r="I25" s="27"/>
+      <c r="J25" s="27"/>
     </row>
-    <row r="26" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="2:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="28" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="22">
+        <v>2</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="2:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="C27" s="14">
+        <v>2</v>
+      </c>
+      <c r="D27" s="26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="2:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1373,15 +1597,15 @@
     <row r="42" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="43" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="44" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="14"/>
-      <c r="C45" s="15"/>
+    <row r="45" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="12"/>
+      <c r="C46" s="13"/>
     </row>
-    <row r="46" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="14"/>
-      <c r="C46" s="15"/>
+    <row r="47" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="12"/>
+      <c r="C47" s="13"/>
     </row>
-    <row r="47" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="48" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2335,12 +2559,23 @@
     <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1001" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="J3:L3"/>
-    <mergeCell ref="F3:H3"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="B14:D14"/>
+  <mergeCells count="14">
+    <mergeCell ref="J23:L23"/>
+    <mergeCell ref="N4:P4"/>
+    <mergeCell ref="B20:U20"/>
+    <mergeCell ref="F8:H8"/>
+    <mergeCell ref="J8:L8"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="F22:H22"/>
+    <mergeCell ref="J4:L4"/>
+    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B2:U2"/>
+    <mergeCell ref="Q4:S4"/>
+    <mergeCell ref="T4:U4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>